<commit_message>
Commit of changes until 2022-04-04
</commit_message>
<xml_diff>
--- a/table/literature.xlsx
+++ b/table/literature.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcblauert/Documents/01_Studium/00_INRM/05_MaThesis/MaThesisWriting/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C346E8D0-6CA8-7A4A-92C0-54F213D0BB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3317CC99-DF71-CF4E-9875-99BCFC32EFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{01F21F64-41ED-7241-89A3-549FD21C02A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{01F21F64-41ED-7241-89A3-549FD21C02A6}"/>
   </bookViews>
   <sheets>
     <sheet name="tab1_literature" sheetId="1" r:id="rId1"/>
+    <sheet name="literature_studies_for_graph" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Study</t>
   </si>
@@ -131,13 +132,37 @@
   </si>
   <si>
     <t>US, household-level (metropolitan areas), panel data, 1995-2007, only single-family homes and duplexes</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Other countries</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,6 +179,14 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -181,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -221,6 +254,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F011FAC9-1914-4E4A-9F4B-698DBC69EB87}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,10 +651,10 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -615,8 +669,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
@@ -700,10 +754,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -718,8 +772,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
@@ -732,10 +786,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -750,8 +804,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
@@ -810,4 +864,215 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C72F86E-984E-8242-8BE1-92B282AA8C4E}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.83203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="17">
+        <v>-0.44</v>
+      </c>
+      <c r="F2" s="16">
+        <v>-0.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="18">
+        <v>-0.31</v>
+      </c>
+      <c r="F3" s="16">
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4">
+        <v>-0.08</v>
+      </c>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4">
+        <v>-0.02</v>
+      </c>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-0.34</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="16">
+        <v>-0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="16">
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-0.48</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="16">
+        <v>-0.71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>